<commit_message>
menambahkan fitur upload gambar di buku_tamu
</commit_message>
<xml_diff>
--- a/Laporan_Buku_Tamu.xlsx
+++ b/Laporan_Buku_Tamu.xlsx
@@ -15,27 +15,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
-    <t>NO</t>
+    <t>2024-10-07</t>
   </si>
   <si>
-    <t>TANGGAL</t>
+    <t>szads</t>
   </si>
   <si>
-    <t>NAMA TAMU</t>
+    <t>dfdfldsfhl</t>
   </si>
   <si>
-    <t>ALAMAT</t>
+    <t>0987654</t>
   </si>
   <si>
-    <t>NO TELEPON/HP</t>
-  </si>
-  <si>
-    <t>BERTEMU DENGAN</t>
-  </si>
-  <si>
-    <t>KEPENTINGAN</t>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -384,26 +378,26 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" t="s">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>